<commit_message>
Rename average_drawdown to average_depth to consistent with average_length & average_recovery
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -786,15 +786,6 @@
     <t>Drawdowns_test1</t>
   </si>
   <si>
-    <t>Average_Drawdown_test</t>
-  </si>
-  <si>
-    <t>Test average drawdown</t>
-  </si>
-  <si>
-    <t>Average Drawdown</t>
-  </si>
-  <si>
     <t>Drawdown_Deviation_test</t>
   </si>
   <si>
@@ -1174,6 +1165,15 @@
   </si>
   <si>
     <t>LPM_test2</t>
+  </si>
+  <si>
+    <t>Average Depth</t>
+  </si>
+  <si>
+    <t>Test average drawdown depth</t>
+  </si>
+  <si>
+    <t>Average_Depth_test</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1500,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,7 +1571,7 @@
         <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1579,24 +1579,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1615,7 +1615,7 @@
         <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C10" t="s">
         <v>164</v>
@@ -1626,7 +1626,7 @@
         <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>382</v>
       </c>
       <c r="B12" t="s">
-        <v>256</v>
+        <v>383</v>
       </c>
       <c r="C12" t="s">
-        <v>255</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1755,13 +1755,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1777,13 +1777,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C25" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
         <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
@@ -1890,7 +1890,7 @@
         <v>168</v>
       </c>
       <c r="B35" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C35" t="s">
         <v>169</v>
@@ -1901,7 +1901,7 @@
         <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C36" t="s">
         <v>170</v>
@@ -1912,7 +1912,7 @@
         <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C37" t="s">
         <v>171</v>
@@ -2385,7 +2385,7 @@
         <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C80" t="s">
         <v>36</v>
@@ -2525,10 +2525,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B93" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C93" t="s">
         <v>46</v>
@@ -2536,24 +2536,24 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B94" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C94" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B95" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C95" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>210</v>
       </c>
       <c r="B96" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C96" t="s">
         <v>40</v>
@@ -2572,7 +2572,7 @@
         <v>214</v>
       </c>
       <c r="B97" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C97" t="s">
         <v>215</v>
@@ -2580,354 +2580,354 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B98" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C98" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B99" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B100" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C100" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B101" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C101" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B102" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C102" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B103" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C103" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B104" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B105" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C105" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B106" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C106" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B107" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C107" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B108" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C108" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B109" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C109" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B110" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C110" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B111" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C111" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B112" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C112" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B113" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C113" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B114" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B115" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C115" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B116" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C116" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>319</v>
+      </c>
+      <c r="B117" t="s">
+        <v>321</v>
+      </c>
+      <c r="C117" t="s">
         <v>322</v>
-      </c>
-      <c r="B117" t="s">
-        <v>324</v>
-      </c>
-      <c r="C117" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>320</v>
+      </c>
+      <c r="B118" t="s">
         <v>323</v>
       </c>
-      <c r="B118" t="s">
-        <v>326</v>
-      </c>
       <c r="C118" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B119" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C119" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B120" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C120" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B121" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C121" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B122" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C122" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B123" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C123" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B124" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C124" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B125" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C125" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B126" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C126" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B127" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C127" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C128" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B129" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C129" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created omega macro, added tests and documentation
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="388">
   <si>
     <t>Test</t>
   </si>
@@ -1174,6 +1174,15 @@
   </si>
   <si>
     <t>Average_Depth_test</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>Test Omega ratio</t>
+  </si>
+  <si>
+    <t>Omega_test</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1498,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1775,7 +1784,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>258</v>
       </c>
@@ -1786,7 +1795,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>242</v>
       </c>
@@ -1797,7 +1806,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -1819,7 +1828,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -1830,7 +1839,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -1852,7 +1861,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>203</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -1885,7 +1894,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -1896,7 +1905,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -1918,7 +1927,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1940,7 +1949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1962,7 +1971,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -2006,7 +2015,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2017,7 +2026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -2050,7 +2059,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2061,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2083,7 +2092,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2094,7 +2103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2116,7 +2125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -2127,7 +2136,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2138,7 +2147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -2149,7 +2158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -2171,7 +2180,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>246</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>212</v>
       </c>
@@ -2215,7 +2224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2237,7 +2246,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -2270,7 +2279,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -2281,7 +2290,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -2292,7 +2301,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>176</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -2314,7 +2323,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>196</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2358,7 +2367,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -2369,7 +2378,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>194</v>
       </c>
@@ -2380,7 +2389,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -2391,7 +2400,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2424,7 +2433,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2446,7 +2455,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>205</v>
       </c>
@@ -2457,7 +2466,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -2468,7 +2477,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -2490,7 +2499,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -2512,7 +2521,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>237</v>
       </c>
@@ -2523,7 +2532,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -2545,7 +2554,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>279</v>
       </c>
@@ -2556,7 +2565,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>210</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>288</v>
       </c>
@@ -2589,7 +2598,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>289</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>292</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>295</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>299</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>301</v>
       </c>
@@ -2644,7 +2653,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>306</v>
       </c>
@@ -2655,7 +2664,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>371</v>
       </c>
@@ -2666,7 +2675,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>345</v>
       </c>
@@ -2677,7 +2686,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>342</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>339</v>
       </c>
@@ -2699,7 +2708,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>336</v>
       </c>
@@ -2710,7 +2719,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>333</v>
       </c>
@@ -2721,7 +2730,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -2732,7 +2741,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>327</v>
       </c>
@@ -2743,7 +2752,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>308</v>
       </c>
@@ -2754,7 +2763,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>309</v>
       </c>
@@ -2765,7 +2774,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>310</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>316</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>319</v>
       </c>
@@ -2798,7 +2807,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>320</v>
       </c>
@@ -2809,7 +2818,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>346</v>
       </c>
@@ -2820,7 +2829,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -2831,7 +2840,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -2842,7 +2851,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>354</v>
       </c>
@@ -2853,7 +2862,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>358</v>
       </c>
@@ -2864,7 +2873,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -2875,7 +2884,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -2886,7 +2895,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -2928,6 +2937,17 @@
       </c>
       <c r="C129" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>385</v>
+      </c>
+      <c r="B130" t="s">
+        <v>386</v>
+      </c>
+      <c r="C130" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Omega_SharpeRatio macro and added tests and documentation
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="391">
   <si>
     <t>Test</t>
   </si>
@@ -1183,6 +1183,15 @@
   </si>
   <si>
     <t>Omega_test</t>
+  </si>
+  <si>
+    <t>Omega Sharpe ratio</t>
+  </si>
+  <si>
+    <t>Test Omega Sharpe ratio</t>
+  </si>
+  <si>
+    <t>Omega_SharpeRatio_test</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1507,7 +1516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B140" sqref="B140"/>
@@ -2950,6 +2959,17 @@
         <v>387</v>
       </c>
     </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>388</v>
+      </c>
+      <c r="B131" t="s">
+        <v>389</v>
+      </c>
+      <c r="C131" t="s">
+        <v>390</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
add test to netselectivity.sas
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\mytest\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="388">
   <si>
     <t>Test</t>
   </si>
@@ -1174,6 +1179,15 @@
   </si>
   <si>
     <t>Average_Depth_test</t>
+  </si>
+  <si>
+    <t>netselectivity</t>
+  </si>
+  <si>
+    <t>Test netselectivity with BM=SPY and Rf=0.05</t>
+  </si>
+  <si>
+    <t>netselectivity_test</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1498,17 +1512,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2809,7 +2823,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>346</v>
       </c>
@@ -2820,7 +2834,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -2831,7 +2845,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -2842,7 +2856,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>354</v>
       </c>
@@ -2853,7 +2867,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>358</v>
       </c>
@@ -2864,7 +2878,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -2875,7 +2889,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -2886,7 +2900,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -2897,7 +2911,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -2908,7 +2922,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>376</v>
       </c>
@@ -2919,7 +2933,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>379</v>
       </c>
@@ -2928,6 +2942,17 @@
       </c>
       <c r="C129" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>385</v>
+      </c>
+      <c r="B130" t="s">
+        <v>386</v>
+      </c>
+      <c r="C130" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "add test to netselectivity.sas"
This reverts commit 330e21897537da19ce45e409a23b62dc8c2de24d.
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\mytest\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="385">
   <si>
     <t>Test</t>
   </si>
@@ -1179,15 +1174,6 @@
   </si>
   <si>
     <t>Average_Depth_test</t>
-  </si>
-  <si>
-    <t>netselectivity</t>
-  </si>
-  <si>
-    <t>Test netselectivity with BM=SPY and Rf=0.05</t>
-  </si>
-  <si>
-    <t>netselectivity_test</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1512,17 +1498,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2823,7 +2809,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>346</v>
       </c>
@@ -2834,7 +2820,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -2845,7 +2831,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -2856,7 +2842,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>354</v>
       </c>
@@ -2867,7 +2853,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>358</v>
       </c>
@@ -2878,7 +2864,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -2889,7 +2875,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -2900,7 +2886,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -2911,7 +2897,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -2922,7 +2908,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>376</v>
       </c>
@@ -2933,7 +2919,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>379</v>
       </c>
@@ -2942,17 +2928,6 @@
       </c>
       <c r="C129" t="s">
         <v>381</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>385</v>
-      </c>
-      <c r="B130" t="s">
-        <v>386</v>
-      </c>
-      <c r="C130" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created OmegaExcessReturn macro and added test and documentation
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="394">
   <si>
     <t>Test</t>
   </si>
@@ -1192,6 +1192,15 @@
   </si>
   <si>
     <t>Omega_SharpeRatio_test</t>
+  </si>
+  <si>
+    <t>Omega Excess return</t>
+  </si>
+  <si>
+    <t>Test Omega Excess return</t>
+  </si>
+  <si>
+    <t>OmegaExcessReturn_test</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1516,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2970,6 +2979,17 @@
         <v>390</v>
       </c>
     </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>391</v>
+      </c>
+      <c r="B132" t="s">
+        <v>392</v>
+      </c>
+      <c r="C132" t="s">
+        <v>393</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Created return_annualized_excess macro and added tests
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="400">
   <si>
     <t>Test</t>
   </si>
@@ -1201,6 +1201,24 @@
   </si>
   <si>
     <t>OmegaExcessReturn_test</t>
+  </si>
+  <si>
+    <t>Test annualized geometric excess return</t>
+  </si>
+  <si>
+    <t>return_annualized_excess_test1</t>
+  </si>
+  <si>
+    <t>return_annualized_excess1</t>
+  </si>
+  <si>
+    <t>return_annualized_excess2</t>
+  </si>
+  <si>
+    <t>Test annualized arithmetic excess return</t>
+  </si>
+  <si>
+    <t>return_annualized_excess_test2</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1525,7 +1543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B138" sqref="B138"/>
@@ -2990,6 +3008,28 @@
         <v>393</v>
       </c>
     </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>396</v>
+      </c>
+      <c r="B133" t="s">
+        <v>394</v>
+      </c>
+      <c r="C133" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>397</v>
+      </c>
+      <c r="B134" t="s">
+        <v>398</v>
+      </c>
+      <c r="C134" t="s">
+        <v>399</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Created Market_Timing macro and added tests and documentation
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="406">
   <si>
     <t>Test</t>
   </si>
@@ -1219,6 +1219,24 @@
   </si>
   <si>
     <t>return_annualized_excess_test2</t>
+  </si>
+  <si>
+    <t>Market Timing1</t>
+  </si>
+  <si>
+    <t>Test market timing with HM model</t>
+  </si>
+  <si>
+    <t>Market_Timing_test1</t>
+  </si>
+  <si>
+    <t>Market Timing2</t>
+  </si>
+  <si>
+    <t>Test market timing with TM model</t>
+  </si>
+  <si>
+    <t>Market_Timing_test2</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1543,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,6 +3048,28 @@
         <v>399</v>
       </c>
     </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>400</v>
+      </c>
+      <c r="B135" t="s">
+        <v>401</v>
+      </c>
+      <c r="C135" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>403</v>
+      </c>
+      <c r="B136" t="s">
+        <v>404</v>
+      </c>
+      <c r="C136" t="s">
+        <v>405</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
test for netselectivity.sas and volatilityskewness.sas in xlsx file
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\SASPerformanceAnalytics\performance_analytics_library\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="414">
   <si>
     <t>Test</t>
   </si>
@@ -1237,6 +1242,30 @@
   </si>
   <si>
     <t>Market_Timing_test2</t>
+  </si>
+  <si>
+    <t>netselectivity</t>
+  </si>
+  <si>
+    <t>Test netselectivity with BM=SPY and Rf=0.05</t>
+  </si>
+  <si>
+    <t>netselectivity_test</t>
+  </si>
+  <si>
+    <t>volatilityskewness</t>
+  </si>
+  <si>
+    <t>Test volatilityskewnsss with option=VOLATILITY</t>
+  </si>
+  <si>
+    <t>volatilityskewness_test1</t>
+  </si>
+  <si>
+    <t>Test volatilityskewnsss with option=VARIABILITY</t>
+  </si>
+  <si>
+    <t>volatilityskewness_test2</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1561,20 +1590,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C136"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1596,7 +1625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1607,7 +1636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1618,7 +1647,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1629,7 +1658,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -1640,7 +1669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>262</v>
       </c>
@@ -1651,7 +1680,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -1662,7 +1691,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -1673,7 +1702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>162</v>
       </c>
@@ -1684,7 +1713,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -1695,7 +1724,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>382</v>
       </c>
@@ -1706,7 +1735,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -1717,7 +1746,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1728,7 +1757,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -1739,7 +1768,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -1750,7 +1779,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -1761,7 +1790,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>225</v>
       </c>
@@ -1772,7 +1801,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1783,7 +1812,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -1794,7 +1823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -1805,7 +1834,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -1816,7 +1845,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>257</v>
       </c>
@@ -1827,7 +1856,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>252</v>
       </c>
@@ -1838,7 +1867,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>258</v>
       </c>
@@ -1849,7 +1878,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>242</v>
       </c>
@@ -1860,7 +1889,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -1871,7 +1900,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -1882,7 +1911,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -1893,7 +1922,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -1904,7 +1933,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -1915,7 +1944,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -1926,7 +1955,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>203</v>
       </c>
@@ -1937,7 +1966,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -1948,7 +1977,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -1959,7 +1988,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -1970,7 +1999,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -1981,7 +2010,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -1992,7 +2021,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -2003,7 +2032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2025,7 +2054,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2036,7 +2065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2047,7 +2076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2058,7 +2087,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -2069,7 +2098,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2080,7 +2109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2091,7 +2120,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -2102,7 +2131,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -2113,7 +2142,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2124,7 +2153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2135,7 +2164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2146,7 +2175,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2157,7 +2186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -2168,7 +2197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2179,7 +2208,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -2190,7 +2219,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2201,7 +2230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -2212,7 +2241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2223,7 +2252,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -2234,7 +2263,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>246</v>
       </c>
@@ -2245,7 +2274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2256,7 +2285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2267,7 +2296,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>212</v>
       </c>
@@ -2278,7 +2307,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -2289,7 +2318,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2300,7 +2329,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2311,7 +2340,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2322,7 +2351,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -2333,7 +2362,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -2344,7 +2373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -2355,7 +2384,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>176</v>
       </c>
@@ -2366,7 +2395,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -2377,7 +2406,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -2388,7 +2417,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>196</v>
       </c>
@@ -2399,7 +2428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -2410,7 +2439,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2421,7 +2450,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -2432,7 +2461,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>194</v>
       </c>
@@ -2443,7 +2472,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -2454,7 +2483,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2465,7 +2494,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -2476,7 +2505,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2487,7 +2516,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2498,7 +2527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2509,7 +2538,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>205</v>
       </c>
@@ -2520,7 +2549,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2542,7 +2571,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -2553,7 +2582,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -2564,7 +2593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -2575,7 +2604,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>237</v>
       </c>
@@ -2586,7 +2615,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -2597,7 +2626,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -2608,7 +2637,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>279</v>
       </c>
@@ -2619,7 +2648,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>210</v>
       </c>
@@ -2630,7 +2659,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -2641,7 +2670,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>288</v>
       </c>
@@ -2652,7 +2681,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>289</v>
       </c>
@@ -2663,7 +2692,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>292</v>
       </c>
@@ -2674,7 +2703,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>295</v>
       </c>
@@ -2685,7 +2714,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>299</v>
       </c>
@@ -2696,7 +2725,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>301</v>
       </c>
@@ -2707,7 +2736,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>306</v>
       </c>
@@ -2718,7 +2747,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>371</v>
       </c>
@@ -2729,7 +2758,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>345</v>
       </c>
@@ -2740,7 +2769,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>342</v>
       </c>
@@ -2751,7 +2780,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>339</v>
       </c>
@@ -2762,7 +2791,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>336</v>
       </c>
@@ -2773,7 +2802,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>333</v>
       </c>
@@ -2784,7 +2813,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -2795,7 +2824,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>327</v>
       </c>
@@ -2806,7 +2835,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>308</v>
       </c>
@@ -2817,7 +2846,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>309</v>
       </c>
@@ -2828,7 +2857,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>310</v>
       </c>
@@ -2839,7 +2868,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>316</v>
       </c>
@@ -2850,7 +2879,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>319</v>
       </c>
@@ -2861,7 +2890,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>320</v>
       </c>
@@ -2872,7 +2901,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>346</v>
       </c>
@@ -2883,7 +2912,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -2894,7 +2923,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -2905,7 +2934,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>354</v>
       </c>
@@ -2916,7 +2945,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>358</v>
       </c>
@@ -2927,7 +2956,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -2938,7 +2967,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -2949,7 +2978,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -2960,7 +2989,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -2971,7 +3000,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>376</v>
       </c>
@@ -2982,7 +3011,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>379</v>
       </c>
@@ -2993,7 +3022,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>385</v>
       </c>
@@ -3004,7 +3033,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>388</v>
       </c>
@@ -3015,7 +3044,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>391</v>
       </c>
@@ -3026,7 +3055,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>396</v>
       </c>
@@ -3037,7 +3066,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>397</v>
       </c>
@@ -3048,7 +3077,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>400</v>
       </c>
@@ -3059,7 +3088,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>403</v>
       </c>
@@ -3068,6 +3097,39 @@
       </c>
       <c r="C136" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>406</v>
+      </c>
+      <c r="B137" t="s">
+        <v>407</v>
+      </c>
+      <c r="C137" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>409</v>
+      </c>
+      <c r="B138" t="s">
+        <v>410</v>
+      </c>
+      <c r="C138" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>409</v>
+      </c>
+      <c r="B139" t="s">
+        <v>412</v>
+      </c>
+      <c r="C139" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tests.xlsx and doc
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\SASPerformanceAnalytics\performance_analytics_library\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="418">
   <si>
     <t>Test</t>
   </si>
@@ -1253,9 +1248,6 @@
     <t>netselectivity_test</t>
   </si>
   <si>
-    <t>volatilityskewness</t>
-  </si>
-  <si>
     <t>Test volatilityskewnsss with option=VOLATILITY</t>
   </si>
   <si>
@@ -1266,6 +1258,21 @@
   </si>
   <si>
     <t>volatilityskewness_test2</t>
+  </si>
+  <si>
+    <t>SkewnessKurtosis ratio</t>
+  </si>
+  <si>
+    <t>Test skewness-kurtosis ratio</t>
+  </si>
+  <si>
+    <t>SkewnessKurtosisRatio_test</t>
+  </si>
+  <si>
+    <t>volatilityskewness1</t>
+  </si>
+  <si>
+    <t>volatilityskewness2</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1590,20 +1597,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:C140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1625,7 +1632,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1647,7 +1654,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1658,7 +1665,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -1669,7 +1676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>262</v>
       </c>
@@ -1680,7 +1687,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -1691,7 +1698,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>162</v>
       </c>
@@ -1713,7 +1720,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -1724,7 +1731,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>382</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -1746,7 +1753,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1757,7 +1764,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -1768,7 +1775,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -1779,7 +1786,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -1790,7 +1797,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>225</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1812,7 +1819,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -1823,7 +1830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -1834,7 +1841,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -1845,7 +1852,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>257</v>
       </c>
@@ -1856,7 +1863,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>252</v>
       </c>
@@ -1867,7 +1874,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>258</v>
       </c>
@@ -1878,7 +1885,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>242</v>
       </c>
@@ -1889,7 +1896,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -1900,7 +1907,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -1911,7 +1918,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -1922,7 +1929,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -1933,7 +1940,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -1944,7 +1951,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -1955,7 +1962,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>203</v>
       </c>
@@ -1966,7 +1973,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -1977,7 +1984,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -1988,7 +1995,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -1999,7 +2006,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -2010,7 +2017,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -2021,7 +2028,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -2032,7 +2039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2054,7 +2061,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2065,7 +2072,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2076,7 +2083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2087,7 +2094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -2098,7 +2105,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2109,7 +2116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2120,7 +2127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -2131,7 +2138,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2153,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2164,7 +2171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2175,7 +2182,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -2197,7 +2204,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2208,7 +2215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -2219,7 +2226,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2252,7 +2259,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -2263,7 +2270,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>246</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2285,7 +2292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2296,7 +2303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>212</v>
       </c>
@@ -2307,7 +2314,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -2318,7 +2325,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2329,7 +2336,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2340,7 +2347,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2351,7 +2358,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -2362,7 +2369,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -2373,7 +2380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -2384,7 +2391,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>176</v>
       </c>
@@ -2395,7 +2402,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -2406,7 +2413,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -2417,7 +2424,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>196</v>
       </c>
@@ -2428,7 +2435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -2439,7 +2446,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -2461,7 +2468,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>194</v>
       </c>
@@ -2472,7 +2479,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -2483,7 +2490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -2505,7 +2512,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2516,7 +2523,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2527,7 +2534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2538,7 +2545,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>205</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -2560,7 +2567,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2571,7 +2578,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -2582,7 +2589,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -2593,7 +2600,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -2604,7 +2611,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>237</v>
       </c>
@@ -2615,7 +2622,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -2626,7 +2633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -2637,7 +2644,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>279</v>
       </c>
@@ -2648,7 +2655,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>210</v>
       </c>
@@ -2659,7 +2666,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -2670,7 +2677,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>288</v>
       </c>
@@ -2681,7 +2688,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>289</v>
       </c>
@@ -2692,7 +2699,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>292</v>
       </c>
@@ -2703,7 +2710,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>295</v>
       </c>
@@ -2714,7 +2721,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>299</v>
       </c>
@@ -2725,7 +2732,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>301</v>
       </c>
@@ -2736,7 +2743,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>306</v>
       </c>
@@ -2747,7 +2754,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>371</v>
       </c>
@@ -2758,7 +2765,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>345</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>342</v>
       </c>
@@ -2780,7 +2787,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>339</v>
       </c>
@@ -2791,7 +2798,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>336</v>
       </c>
@@ -2802,7 +2809,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>333</v>
       </c>
@@ -2813,7 +2820,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -2824,7 +2831,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>327</v>
       </c>
@@ -2835,7 +2842,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>308</v>
       </c>
@@ -2846,7 +2853,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>309</v>
       </c>
@@ -2857,7 +2864,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>310</v>
       </c>
@@ -2868,7 +2875,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>316</v>
       </c>
@@ -2879,7 +2886,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>319</v>
       </c>
@@ -2890,7 +2897,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>320</v>
       </c>
@@ -2901,7 +2908,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>346</v>
       </c>
@@ -2912,7 +2919,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -2923,7 +2930,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>354</v>
       </c>
@@ -2945,7 +2952,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>358</v>
       </c>
@@ -2956,7 +2963,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -2967,7 +2974,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -2978,7 +2985,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -3000,7 +3007,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>376</v>
       </c>
@@ -3011,7 +3018,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>379</v>
       </c>
@@ -3022,7 +3029,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>385</v>
       </c>
@@ -3033,7 +3040,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>388</v>
       </c>
@@ -3044,7 +3051,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>391</v>
       </c>
@@ -3055,7 +3062,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>396</v>
       </c>
@@ -3066,7 +3073,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>397</v>
       </c>
@@ -3077,7 +3084,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>400</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>403</v>
       </c>
@@ -3099,7 +3106,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>406</v>
       </c>
@@ -3110,26 +3117,37 @@
         <v>408</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>416</v>
+      </c>
+      <c r="B138" t="s">
         <v>409</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>410</v>
       </c>
-      <c r="C138" t="s">
+    </row>
+    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>417</v>
+      </c>
+      <c r="B139" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>409</v>
-      </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>412</v>
       </c>
-      <c r="C139" t="s">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>413</v>
+      </c>
+      <c r="B140" t="s">
+        <v>414</v>
+      </c>
+      <c r="C140" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created return_relative and added tests and documentation
</commit_message>
<xml_diff>
--- a/performance_analytics_library/test/tests.xlsx
+++ b/performance_analytics_library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="421">
   <si>
     <t>Test</t>
   </si>
@@ -1273,6 +1273,15 @@
   </si>
   <si>
     <t>volatilityskewness2</t>
+  </si>
+  <si>
+    <t>return_relative</t>
+  </si>
+  <si>
+    <t>Test return_relative for simple returns</t>
+  </si>
+  <si>
+    <t>return_relative_test</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1597,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3150,6 +3159,17 @@
         <v>415</v>
       </c>
     </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>418</v>
+      </c>
+      <c r="B141" t="s">
+        <v>419</v>
+      </c>
+      <c r="C141" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>